<commit_message>
meest recente bestanden teruggezet
</commit_message>
<xml_diff>
--- a/pbelasting/input/160706_giab.xlsx
+++ b/pbelasting/input/160706_giab.xlsx
@@ -37874,10 +37874,10 @@
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Classificatie xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Intern</Classificatie>
-    <_dlc_DocId xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">PNHZET2ZRHHM-1647798991-93063</_dlc_DocId>
+    <_dlc_DocId xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">PNHZET2ZRHHM-1647798991-177039</_dlc_DocId>
     <_dlc_DocIdUrl xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">
-      <Url>https://waternet.sharepoint.com/sites/0182/_layouts/15/DocIdRedir.aspx?ID=PNHZET2ZRHHM-1647798991-93063</Url>
-      <Description>PNHZET2ZRHHM-1647798991-93063</Description>
+      <Url>https://waternet.sharepoint.com/sites/0182/_layouts/15/DocIdRedir.aspx?ID=PNHZET2ZRHHM-1647798991-177039</Url>
+      <Description>PNHZET2ZRHHM-1647798991-177039</Description>
     </_dlc_DocIdUrl>
     <Aggregatieniveau xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Archiefstuk</Aggregatieniveau>
     <Identificatiekenmerk xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>

</xml_diff>